<commit_message>
Updated utility PV potential; updated PHS VOM cost; updated TYNDP link carriers
</commit_message>
<xml_diff>
--- a/src/parameters/tech_info.xlsx
+++ b/src/parameters/tech_info.xlsx
@@ -852,7 +852,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1076,13 +1076,13 @@
         <v>23</v>
       </c>
       <c r="C8" s="2">
-        <v>4000</v>
+        <v>2880</v>
       </c>
       <c r="D8" s="2">
-        <v>10.5</v>
+        <v>14.3</v>
       </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>2.5000000000000002E-6</v>
       </c>
       <c r="G8" s="4">
         <v>0.9</v>

</xml_diff>

<commit_message>
Cost calculation updated (more decimals)
</commit_message>
<xml_diff>
--- a/src/parameters/tech_info.xlsx
+++ b/src/parameters/tech_info.xlsx
@@ -261,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -367,6 +367,13 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -475,7 +482,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,6 +491,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent 1 17" xfId="1"/>
@@ -852,7 +861,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -1082,7 +1091,7 @@
         <v>14.3</v>
       </c>
       <c r="E8" s="2">
-        <v>2.5000000000000002E-6</v>
+        <v>2.2500000000000001E-6</v>
       </c>
       <c r="G8" s="4">
         <v>0.9</v>
@@ -1114,7 +1123,7 @@
         <v>36</v>
       </c>
       <c r="E9" s="2">
-        <v>2.7000000000000001E-3</v>
+        <v>2.7E-4</v>
       </c>
       <c r="G9" s="4">
         <v>0.95</v>
@@ -1162,8 +1171,8 @@
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11">
-        <v>2200</v>
+      <c r="C11" s="6">
+        <v>2000</v>
       </c>
       <c r="D11">
         <v>33.200000000000003</v>
@@ -1212,10 +1221,10 @@
         <v>500</v>
       </c>
       <c r="D13">
-        <v>6.6</v>
-      </c>
-      <c r="E13" s="3">
         <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.8E-3</v>
       </c>
       <c r="L13">
         <v>25</v>
@@ -1231,14 +1240,14 @@
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>800</v>
+      <c r="C14" s="6">
+        <v>700</v>
       </c>
       <c r="D14">
-        <v>7.8</v>
-      </c>
-      <c r="E14" s="3">
         <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.8E-3</v>
       </c>
       <c r="L14">
         <v>25</v>

</xml_diff>

<commit_message>
Updated wind CF computation.
</commit_message>
<xml_diff>
--- a/src/parameters/tech_info.xlsx
+++ b/src/parameters/tech_info.xlsx
@@ -861,14 +861,14 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11.5"/>
     <col min="2" max="2" width="14.0546875" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" customWidth="1"/>
     <col min="4" max="4" width="6.44140625" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>

</xml_diff>